<commit_message>
commit changed pom 3
</commit_message>
<xml_diff>
--- a/Display_Bookshelves/BookshelvesDetails.xlsx
+++ b/Display_Bookshelves/BookshelvesDetails.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -23,6 +23,18 @@
     <t>Price (Rs)</t>
   </si>
   <si>
+    <t>Rhodes Folding Book Shelf</t>
+  </si>
+  <si>
+    <t>(Teak Finish, Tall Configuration, 60 Book Book Capacity)</t>
+  </si>
+  <si>
+    <t>₹15,599</t>
+  </si>
+  <si>
+    <t>(Mahogany Finish, Tall Configuration, 60 Book Book Capacity)</t>
+  </si>
+  <si>
     <t>Austen Bookshelf/Display Unit</t>
   </si>
   <si>
@@ -53,16 +65,16 @@
     <t>₹1,699 ₹1,019</t>
   </si>
   <si>
+    <t>(Dark Walnut Finish)</t>
+  </si>
+  <si>
+    <t>₹1,499 ₹899</t>
+  </si>
+  <si>
     <t>Boeberg Drawer Inserts</t>
   </si>
   <si>
     <t>₹2,699 ₹1,619</t>
-  </si>
-  <si>
-    <t>(Dark Walnut Finish)</t>
-  </si>
-  <si>
-    <t>₹1,499 ₹899</t>
   </si>
 </sst>
 </file>
@@ -107,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -159,35 +171,57 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>